<commit_message>
Se agrega modal de firma
</commit_message>
<xml_diff>
--- a/Referencia.xlsx
+++ b/Referencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Proyecto Infotrack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D305EDD1-ED18-4635-9C69-4D9175B8A4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441E9356-B11E-4F69-95AD-EB58262EE7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="8532" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>LISTA DE CHEQUEO - HAND HELD. (Recepción)</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t>{{ID_CLIENTE}}</t>
+  </si>
+  <si>
+    <t>{{NOMBRE_ENTREGA}}</t>
+  </si>
+  <si>
+    <t>{{CEDULA_ENTREGA}}</t>
   </si>
 </sst>
 </file>
@@ -636,7 +642,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -679,9 +685,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -710,26 +713,31 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -754,26 +762,20 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="33" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1161,32 +1163,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IW41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="43" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="43" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37:O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="16.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="56.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.88671875" style="1" customWidth="1"/>
-    <col min="5" max="18" width="8.109375" style="1" customWidth="1"/>
-    <col min="19" max="20" width="8.5546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="20.5546875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.44140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="12.33203125" style="1" customWidth="1"/>
-    <col min="24" max="25" width="14.44140625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="26.5546875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="33.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" style="1" customWidth="1"/>
+    <col min="5" max="18" width="8.140625" style="1" customWidth="1"/>
+    <col min="19" max="20" width="8.5703125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="1" customWidth="1"/>
+    <col min="24" max="25" width="14.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="26.5703125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="33.28515625" style="1" customWidth="1"/>
     <col min="28" max="257" width="12" style="1" customWidth="1"/>
     <col min="258" max="258" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="79.5" customHeight="1">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="A1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="41" t="s">
         <v>0</v>
       </c>
@@ -1280,13 +1282,13 @@
       <c r="A5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="45" t="s">
@@ -1306,24 +1308,24 @@
       <c r="Q5" s="45"/>
       <c r="R5" s="45"/>
       <c r="S5" s="45"/>
-      <c r="T5" s="40" t="s">
+      <c r="T5" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="U5" s="40"/>
-      <c r="V5" s="40"/>
-      <c r="W5" s="40"/>
-      <c r="X5" s="40"/>
-      <c r="Y5" s="40"/>
-      <c r="Z5" s="40"/>
-      <c r="AA5" s="40"/>
+      <c r="U5" s="39"/>
+      <c r="V5" s="39"/>
+      <c r="W5" s="39"/>
+      <c r="X5" s="39"/>
+      <c r="Y5" s="39"/>
+      <c r="Z5" s="39"/>
+      <c r="AA5" s="39"/>
       <c r="AB5" s="5"/>
       <c r="AC5" s="6"/>
     </row>
     <row r="6" spans="1:29" ht="188.25" customHeight="1">
       <c r="A6" s="43"/>
       <c r="B6" s="44"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="7" t="s">
         <v>12</v>
       </c>
@@ -1369,1799 +1371,1799 @@
       <c r="S6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="40"/>
-      <c r="U6" s="40"/>
-      <c r="V6" s="40"/>
-      <c r="W6" s="40"/>
-      <c r="X6" s="40"/>
-      <c r="Y6" s="40"/>
-      <c r="Z6" s="40"/>
-      <c r="AA6" s="40"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="39"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="39"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="39"/>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="39"/>
       <c r="AB6" s="9"/>
       <c r="AC6" s="6"/>
     </row>
     <row r="7" spans="1:29" ht="138" customHeight="1">
-      <c r="A7" s="28">
+      <c r="A7" s="27">
         <v>1</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="30" t="str">
+      <c r="C7" s="29" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_SERIAL}}"</f>
         <v>{{E1_SERIAL}}</v>
       </c>
-      <c r="D7" s="25" t="str">
+      <c r="D7" s="24" t="str">
         <f>"{{E" &amp; ROW(D7) - 6 &amp; "_MODELO}}"</f>
         <v>{{E1_MODELO}}</v>
       </c>
-      <c r="E7" s="26" t="str">
+      <c r="E7" s="25" t="str">
         <f>"{{E" &amp; ROW(E7) - 6 &amp; "_LAPIZ}}"</f>
         <v>{{E1_LAPIZ}}</v>
       </c>
-      <c r="F7" s="26" t="str">
+      <c r="F7" s="25" t="str">
         <f>"{{E" &amp; ROW(F7) - 6 &amp; "_CUERDA}}"</f>
         <v>{{E1_CUERDA}}</v>
       </c>
-      <c r="G7" s="26" t="str">
+      <c r="G7" s="25" t="str">
         <f>"{{E" &amp; ROW(G7) - 6 &amp; "_CORREA}}"</f>
         <v>{{E1_CORREA}}</v>
       </c>
-      <c r="H7" s="26" t="str">
+      <c r="H7" s="25" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_TECLADO_NUM}}"</f>
         <v>{{E1_TECLADO_NUM}}</v>
       </c>
-      <c r="I7" s="26" t="str">
+      <c r="I7" s="25" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_TECLADO_COMPL}}"</f>
         <v>{{E1_TECLADO_COMPL}}</v>
       </c>
-      <c r="J7" s="26" t="str">
+      <c r="J7" s="25" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_PANTALLA}}"</f>
         <v>{{E1_PANTALLA}}</v>
       </c>
-      <c r="K7" s="27" t="str">
+      <c r="K7" s="26" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_PROTECTOR}}"</f>
         <v>{{E1_PROTECTOR}}</v>
       </c>
-      <c r="L7" s="26" t="str">
+      <c r="L7" s="25" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_BATERIA}}"</f>
         <v>{{E1_BATERIA}}</v>
       </c>
-      <c r="M7" s="26" t="str">
+      <c r="M7" s="25" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_TAPA_BATERIA}}"</f>
         <v>{{E1_TAPA_BATERIA}}</v>
       </c>
-      <c r="N7" s="26" t="str">
+      <c r="N7" s="25" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_TARJETA_ALM}}"</f>
         <v>{{E1_TARJETA_ALM}}</v>
       </c>
-      <c r="O7" s="26" t="str">
+      <c r="O7" s="25" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_CUBIERTA_TARJETA}}"</f>
         <v>{{E1_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P7" s="26" t="str">
+      <c r="P7" s="25" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_CRISTAL}}"</f>
         <v>{{E1_CRISTAL}}</v>
       </c>
-      <c r="Q7" s="26" t="str">
+      <c r="Q7" s="25" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_CARCAZA_SUP}}"</f>
         <v>{{E1_CARCAZA_SUP}}</v>
       </c>
-      <c r="R7" s="26" t="str">
+      <c r="R7" s="25" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_CARCAZA_INF}}"</f>
         <v>{{E1_CARCAZA_INF}}</v>
       </c>
-      <c r="S7" s="26" t="str">
+      <c r="S7" s="25" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_SIM}}"</f>
         <v>{{E1_SIM}}</v>
       </c>
-      <c r="T7" s="49" t="str">
+      <c r="T7" s="32" t="str">
         <f>"{{E" &amp; ROW(C7) - 6 &amp; "_PROBLEMA}}"</f>
         <v>{{E1_PROBLEMA}}</v>
       </c>
-      <c r="U7" s="50"/>
-      <c r="V7" s="50"/>
-      <c r="W7" s="50"/>
-      <c r="X7" s="50"/>
-      <c r="Y7" s="50"/>
-      <c r="Z7" s="50"/>
-      <c r="AA7" s="51"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="33"/>
+      <c r="AA7" s="34"/>
       <c r="AB7" s="9"/>
       <c r="AC7" s="6"/>
     </row>
     <row r="8" spans="1:29" ht="138" customHeight="1">
-      <c r="A8" s="28">
+      <c r="A8" s="27">
         <v>2</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="30" t="str">
+      <c r="C8" s="29" t="str">
         <f t="shared" ref="C8:C26" si="0">"{{E" &amp; ROW(C8) - 6 &amp; "_SERIAL}}"</f>
         <v>{{E2_SERIAL}}</v>
       </c>
-      <c r="D8" s="25" t="str">
+      <c r="D8" s="24" t="str">
         <f t="shared" ref="D8:D26" si="1">"{{E" &amp; ROW(D8) - 6 &amp; "_MODELO}}"</f>
         <v>{{E2_MODELO}}</v>
       </c>
-      <c r="E8" s="26" t="str">
+      <c r="E8" s="25" t="str">
         <f t="shared" ref="E8:E26" si="2">"{{E" &amp; ROW(E8) - 6 &amp; "_LAPIZ}}"</f>
         <v>{{E2_LAPIZ}}</v>
       </c>
-      <c r="F8" s="26" t="str">
+      <c r="F8" s="25" t="str">
         <f t="shared" ref="F8:F26" si="3">"{{E" &amp; ROW(F8) - 6 &amp; "_CUERDA}}"</f>
         <v>{{E2_CUERDA}}</v>
       </c>
-      <c r="G8" s="26" t="str">
+      <c r="G8" s="25" t="str">
         <f t="shared" ref="G8:G26" si="4">"{{E" &amp; ROW(G8) - 6 &amp; "_CORREA}}"</f>
         <v>{{E2_CORREA}}</v>
       </c>
-      <c r="H8" s="26" t="str">
+      <c r="H8" s="25" t="str">
         <f t="shared" ref="H8:H26" si="5">"{{E" &amp; ROW(C8) - 6 &amp; "_TECLADO_NUM}}"</f>
         <v>{{E2_TECLADO_NUM}}</v>
       </c>
-      <c r="I8" s="26" t="str">
+      <c r="I8" s="25" t="str">
         <f t="shared" ref="I8:I26" si="6">"{{E" &amp; ROW(C8) - 6 &amp; "_TECLADO_COMPL}}"</f>
         <v>{{E2_TECLADO_COMPL}}</v>
       </c>
-      <c r="J8" s="26" t="str">
+      <c r="J8" s="25" t="str">
         <f t="shared" ref="J8:J26" si="7">"{{E" &amp; ROW(C8) - 6 &amp; "_PANTALLA}}"</f>
         <v>{{E2_PANTALLA}}</v>
       </c>
-      <c r="K8" s="27" t="str">
+      <c r="K8" s="26" t="str">
         <f t="shared" ref="K8:K26" si="8">"{{E" &amp; ROW(C8) - 6 &amp; "_PROTECTOR}}"</f>
         <v>{{E2_PROTECTOR}}</v>
       </c>
-      <c r="L8" s="26" t="str">
+      <c r="L8" s="25" t="str">
         <f t="shared" ref="L8:L26" si="9">"{{E" &amp; ROW(C8) - 6 &amp; "_BATERIA}}"</f>
         <v>{{E2_BATERIA}}</v>
       </c>
-      <c r="M8" s="26" t="str">
+      <c r="M8" s="25" t="str">
         <f t="shared" ref="M8:M26" si="10">"{{E" &amp; ROW(C8) - 6 &amp; "_TAPA_BATERIA}}"</f>
         <v>{{E2_TAPA_BATERIA}}</v>
       </c>
-      <c r="N8" s="26" t="str">
+      <c r="N8" s="25" t="str">
         <f t="shared" ref="N8:N26" si="11">"{{E" &amp; ROW(C8) - 6 &amp; "_TARJETA_ALM}}"</f>
         <v>{{E2_TARJETA_ALM}}</v>
       </c>
-      <c r="O8" s="26" t="str">
+      <c r="O8" s="25" t="str">
         <f t="shared" ref="O8:O26" si="12">"{{E" &amp; ROW(C8) - 6 &amp; "_CUBIERTA_TARJETA}}"</f>
         <v>{{E2_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P8" s="26" t="str">
+      <c r="P8" s="25" t="str">
         <f t="shared" ref="P8:P26" si="13">"{{E" &amp; ROW(C8) - 6 &amp; "_CRISTAL}}"</f>
         <v>{{E2_CRISTAL}}</v>
       </c>
-      <c r="Q8" s="26" t="str">
+      <c r="Q8" s="25" t="str">
         <f t="shared" ref="Q8:Q26" si="14">"{{E" &amp; ROW(C8) - 6 &amp; "_CARCAZA_SUP}}"</f>
         <v>{{E2_CARCAZA_SUP}}</v>
       </c>
-      <c r="R8" s="26" t="str">
+      <c r="R8" s="25" t="str">
         <f t="shared" ref="R8:R26" si="15">"{{E" &amp; ROW(C8) - 6 &amp; "_CARCAZA_INF}}"</f>
         <v>{{E2_CARCAZA_INF}}</v>
       </c>
-      <c r="S8" s="26" t="str">
+      <c r="S8" s="25" t="str">
         <f t="shared" ref="S8:S26" si="16">"{{E" &amp; ROW(C8) - 6 &amp; "_SIM}}"</f>
         <v>{{E2_SIM}}</v>
       </c>
-      <c r="T8" s="49" t="str">
+      <c r="T8" s="32" t="str">
         <f t="shared" ref="T8:T26" si="17">"{{E" &amp; ROW(C8) - 6 &amp; "_PROBLEMA}}"</f>
         <v>{{E2_PROBLEMA}}</v>
       </c>
-      <c r="U8" s="50"/>
-      <c r="V8" s="50"/>
-      <c r="W8" s="50"/>
-      <c r="X8" s="50"/>
-      <c r="Y8" s="50"/>
-      <c r="Z8" s="50"/>
-      <c r="AA8" s="51"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="33"/>
+      <c r="W8" s="33"/>
+      <c r="X8" s="33"/>
+      <c r="Y8" s="33"/>
+      <c r="Z8" s="33"/>
+      <c r="AA8" s="34"/>
       <c r="AB8" s="9"/>
       <c r="AC8" s="6"/>
     </row>
     <row r="9" spans="1:29" ht="138" customHeight="1">
-      <c r="A9" s="28">
+      <c r="A9" s="27">
         <v>3</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="30" t="str">
+      <c r="C9" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E3_SERIAL}}</v>
       </c>
-      <c r="D9" s="25" t="str">
+      <c r="D9" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E3_MODELO}}</v>
       </c>
-      <c r="E9" s="26" t="str">
+      <c r="E9" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E3_LAPIZ}}</v>
       </c>
-      <c r="F9" s="26" t="str">
+      <c r="F9" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E3_CUERDA}}</v>
       </c>
-      <c r="G9" s="26" t="str">
+      <c r="G9" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E3_CORREA}}</v>
       </c>
-      <c r="H9" s="26" t="str">
+      <c r="H9" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E3_TECLADO_NUM}}</v>
       </c>
-      <c r="I9" s="26" t="str">
+      <c r="I9" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E3_TECLADO_COMPL}}</v>
       </c>
-      <c r="J9" s="26" t="str">
+      <c r="J9" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E3_PANTALLA}}</v>
       </c>
-      <c r="K9" s="27" t="str">
+      <c r="K9" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E3_PROTECTOR}}</v>
       </c>
-      <c r="L9" s="26" t="str">
+      <c r="L9" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E3_BATERIA}}</v>
       </c>
-      <c r="M9" s="26" t="str">
+      <c r="M9" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E3_TAPA_BATERIA}}</v>
       </c>
-      <c r="N9" s="26" t="str">
+      <c r="N9" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E3_TARJETA_ALM}}</v>
       </c>
-      <c r="O9" s="26" t="str">
+      <c r="O9" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E3_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P9" s="26" t="str">
+      <c r="P9" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E3_CRISTAL}}</v>
       </c>
-      <c r="Q9" s="26" t="str">
+      <c r="Q9" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E3_CARCAZA_SUP}}</v>
       </c>
-      <c r="R9" s="26" t="str">
+      <c r="R9" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E3_CARCAZA_INF}}</v>
       </c>
-      <c r="S9" s="26" t="str">
+      <c r="S9" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E3_SIM}}</v>
       </c>
-      <c r="T9" s="49" t="str">
+      <c r="T9" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E3_PROBLEMA}}</v>
       </c>
-      <c r="U9" s="50"/>
-      <c r="V9" s="50"/>
-      <c r="W9" s="50"/>
-      <c r="X9" s="50"/>
-      <c r="Y9" s="50"/>
-      <c r="Z9" s="50"/>
-      <c r="AA9" s="51"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="33"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="33"/>
+      <c r="Z9" s="33"/>
+      <c r="AA9" s="34"/>
       <c r="AB9" s="9"/>
       <c r="AC9" s="6"/>
     </row>
     <row r="10" spans="1:29" ht="138" customHeight="1">
-      <c r="A10" s="28">
+      <c r="A10" s="27">
         <v>4</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="30" t="str">
+      <c r="C10" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E4_SERIAL}}</v>
       </c>
-      <c r="D10" s="25" t="str">
+      <c r="D10" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E4_MODELO}}</v>
       </c>
-      <c r="E10" s="26" t="str">
+      <c r="E10" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E4_LAPIZ}}</v>
       </c>
-      <c r="F10" s="26" t="str">
+      <c r="F10" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E4_CUERDA}}</v>
       </c>
-      <c r="G10" s="26" t="str">
+      <c r="G10" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E4_CORREA}}</v>
       </c>
-      <c r="H10" s="26" t="str">
+      <c r="H10" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E4_TECLADO_NUM}}</v>
       </c>
-      <c r="I10" s="26" t="str">
+      <c r="I10" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E4_TECLADO_COMPL}}</v>
       </c>
-      <c r="J10" s="26" t="str">
+      <c r="J10" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E4_PANTALLA}}</v>
       </c>
-      <c r="K10" s="27" t="str">
+      <c r="K10" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E4_PROTECTOR}}</v>
       </c>
-      <c r="L10" s="26" t="str">
+      <c r="L10" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E4_BATERIA}}</v>
       </c>
-      <c r="M10" s="26" t="str">
+      <c r="M10" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E4_TAPA_BATERIA}}</v>
       </c>
-      <c r="N10" s="26" t="str">
+      <c r="N10" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E4_TARJETA_ALM}}</v>
       </c>
-      <c r="O10" s="26" t="str">
+      <c r="O10" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E4_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P10" s="26" t="str">
+      <c r="P10" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E4_CRISTAL}}</v>
       </c>
-      <c r="Q10" s="26" t="str">
+      <c r="Q10" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E4_CARCAZA_SUP}}</v>
       </c>
-      <c r="R10" s="26" t="str">
+      <c r="R10" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E4_CARCAZA_INF}}</v>
       </c>
-      <c r="S10" s="26" t="str">
+      <c r="S10" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E4_SIM}}</v>
       </c>
-      <c r="T10" s="49" t="str">
+      <c r="T10" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E4_PROBLEMA}}</v>
       </c>
-      <c r="U10" s="50"/>
-      <c r="V10" s="50"/>
-      <c r="W10" s="50"/>
-      <c r="X10" s="50"/>
-      <c r="Y10" s="50"/>
-      <c r="Z10" s="50"/>
-      <c r="AA10" s="51"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
+      <c r="X10" s="33"/>
+      <c r="Y10" s="33"/>
+      <c r="Z10" s="33"/>
+      <c r="AA10" s="34"/>
       <c r="AB10" s="9"/>
       <c r="AC10" s="6"/>
     </row>
     <row r="11" spans="1:29" ht="138" customHeight="1">
-      <c r="A11" s="28">
+      <c r="A11" s="27">
         <v>5</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="30" t="str">
+      <c r="C11" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E5_SERIAL}}</v>
       </c>
-      <c r="D11" s="25" t="str">
+      <c r="D11" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E5_MODELO}}</v>
       </c>
-      <c r="E11" s="26" t="str">
+      <c r="E11" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E5_LAPIZ}}</v>
       </c>
-      <c r="F11" s="26" t="str">
+      <c r="F11" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E5_CUERDA}}</v>
       </c>
-      <c r="G11" s="26" t="str">
+      <c r="G11" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E5_CORREA}}</v>
       </c>
-      <c r="H11" s="26" t="str">
+      <c r="H11" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E5_TECLADO_NUM}}</v>
       </c>
-      <c r="I11" s="26" t="str">
+      <c r="I11" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E5_TECLADO_COMPL}}</v>
       </c>
-      <c r="J11" s="26" t="str">
+      <c r="J11" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E5_PANTALLA}}</v>
       </c>
-      <c r="K11" s="27" t="str">
+      <c r="K11" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E5_PROTECTOR}}</v>
       </c>
-      <c r="L11" s="26" t="str">
+      <c r="L11" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E5_BATERIA}}</v>
       </c>
-      <c r="M11" s="26" t="str">
+      <c r="M11" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E5_TAPA_BATERIA}}</v>
       </c>
-      <c r="N11" s="26" t="str">
+      <c r="N11" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E5_TARJETA_ALM}}</v>
       </c>
-      <c r="O11" s="26" t="str">
+      <c r="O11" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E5_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P11" s="26" t="str">
+      <c r="P11" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E5_CRISTAL}}</v>
       </c>
-      <c r="Q11" s="26" t="str">
+      <c r="Q11" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E5_CARCAZA_SUP}}</v>
       </c>
-      <c r="R11" s="26" t="str">
+      <c r="R11" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E5_CARCAZA_INF}}</v>
       </c>
-      <c r="S11" s="26" t="str">
+      <c r="S11" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E5_SIM}}</v>
       </c>
-      <c r="T11" s="49" t="str">
+      <c r="T11" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E5_PROBLEMA}}</v>
       </c>
-      <c r="U11" s="50"/>
-      <c r="V11" s="50"/>
-      <c r="W11" s="50"/>
-      <c r="X11" s="50"/>
-      <c r="Y11" s="50"/>
-      <c r="Z11" s="50"/>
-      <c r="AA11" s="51"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
+      <c r="X11" s="33"/>
+      <c r="Y11" s="33"/>
+      <c r="Z11" s="33"/>
+      <c r="AA11" s="34"/>
       <c r="AB11" s="9"/>
       <c r="AC11" s="6"/>
     </row>
     <row r="12" spans="1:29" ht="138" customHeight="1">
-      <c r="A12" s="28">
+      <c r="A12" s="27">
         <v>6</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="30" t="str">
+      <c r="C12" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E6_SERIAL}}</v>
       </c>
-      <c r="D12" s="25" t="str">
+      <c r="D12" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E6_MODELO}}</v>
       </c>
-      <c r="E12" s="26" t="str">
+      <c r="E12" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E6_LAPIZ}}</v>
       </c>
-      <c r="F12" s="26" t="str">
+      <c r="F12" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E6_CUERDA}}</v>
       </c>
-      <c r="G12" s="26" t="str">
+      <c r="G12" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E6_CORREA}}</v>
       </c>
-      <c r="H12" s="26" t="str">
+      <c r="H12" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E6_TECLADO_NUM}}</v>
       </c>
-      <c r="I12" s="26" t="str">
+      <c r="I12" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E6_TECLADO_COMPL}}</v>
       </c>
-      <c r="J12" s="26" t="str">
+      <c r="J12" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E6_PANTALLA}}</v>
       </c>
-      <c r="K12" s="27" t="str">
+      <c r="K12" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E6_PROTECTOR}}</v>
       </c>
-      <c r="L12" s="26" t="str">
+      <c r="L12" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E6_BATERIA}}</v>
       </c>
-      <c r="M12" s="26" t="str">
+      <c r="M12" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E6_TAPA_BATERIA}}</v>
       </c>
-      <c r="N12" s="26" t="str">
+      <c r="N12" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E6_TARJETA_ALM}}</v>
       </c>
-      <c r="O12" s="26" t="str">
+      <c r="O12" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E6_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P12" s="26" t="str">
+      <c r="P12" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E6_CRISTAL}}</v>
       </c>
-      <c r="Q12" s="26" t="str">
+      <c r="Q12" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E6_CARCAZA_SUP}}</v>
       </c>
-      <c r="R12" s="26" t="str">
+      <c r="R12" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E6_CARCAZA_INF}}</v>
       </c>
-      <c r="S12" s="26" t="str">
+      <c r="S12" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E6_SIM}}</v>
       </c>
-      <c r="T12" s="49" t="str">
+      <c r="T12" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E6_PROBLEMA}}</v>
       </c>
-      <c r="U12" s="50"/>
-      <c r="V12" s="50"/>
-      <c r="W12" s="50"/>
-      <c r="X12" s="50"/>
-      <c r="Y12" s="50"/>
-      <c r="Z12" s="50"/>
-      <c r="AA12" s="51"/>
+      <c r="U12" s="33"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="33"/>
+      <c r="Y12" s="33"/>
+      <c r="Z12" s="33"/>
+      <c r="AA12" s="34"/>
       <c r="AB12" s="9"/>
       <c r="AC12" s="6"/>
     </row>
     <row r="13" spans="1:29" ht="138" customHeight="1">
-      <c r="A13" s="28">
+      <c r="A13" s="27">
         <v>7</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="30" t="str">
+      <c r="C13" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E7_SERIAL}}</v>
       </c>
-      <c r="D13" s="25" t="str">
+      <c r="D13" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E7_MODELO}}</v>
       </c>
-      <c r="E13" s="26" t="str">
+      <c r="E13" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E7_LAPIZ}}</v>
       </c>
-      <c r="F13" s="26" t="str">
+      <c r="F13" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E7_CUERDA}}</v>
       </c>
-      <c r="G13" s="26" t="str">
+      <c r="G13" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E7_CORREA}}</v>
       </c>
-      <c r="H13" s="26" t="str">
+      <c r="H13" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E7_TECLADO_NUM}}</v>
       </c>
-      <c r="I13" s="26" t="str">
+      <c r="I13" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E7_TECLADO_COMPL}}</v>
       </c>
-      <c r="J13" s="26" t="str">
+      <c r="J13" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E7_PANTALLA}}</v>
       </c>
-      <c r="K13" s="27" t="str">
+      <c r="K13" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E7_PROTECTOR}}</v>
       </c>
-      <c r="L13" s="26" t="str">
+      <c r="L13" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E7_BATERIA}}</v>
       </c>
-      <c r="M13" s="26" t="str">
+      <c r="M13" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E7_TAPA_BATERIA}}</v>
       </c>
-      <c r="N13" s="26" t="str">
+      <c r="N13" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E7_TARJETA_ALM}}</v>
       </c>
-      <c r="O13" s="26" t="str">
+      <c r="O13" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E7_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P13" s="26" t="str">
+      <c r="P13" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E7_CRISTAL}}</v>
       </c>
-      <c r="Q13" s="26" t="str">
+      <c r="Q13" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E7_CARCAZA_SUP}}</v>
       </c>
-      <c r="R13" s="26" t="str">
+      <c r="R13" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E7_CARCAZA_INF}}</v>
       </c>
-      <c r="S13" s="26" t="str">
+      <c r="S13" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E7_SIM}}</v>
       </c>
-      <c r="T13" s="49" t="str">
+      <c r="T13" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E7_PROBLEMA}}</v>
       </c>
-      <c r="U13" s="50"/>
-      <c r="V13" s="50"/>
-      <c r="W13" s="50"/>
-      <c r="X13" s="50"/>
-      <c r="Y13" s="50"/>
-      <c r="Z13" s="50"/>
-      <c r="AA13" s="51"/>
+      <c r="U13" s="33"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="33"/>
+      <c r="Y13" s="33"/>
+      <c r="Z13" s="33"/>
+      <c r="AA13" s="34"/>
       <c r="AB13" s="9"/>
       <c r="AC13" s="6"/>
     </row>
     <row r="14" spans="1:29" ht="138" customHeight="1">
-      <c r="A14" s="28">
+      <c r="A14" s="27">
         <v>8</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="30" t="str">
+      <c r="C14" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E8_SERIAL}}</v>
       </c>
-      <c r="D14" s="25" t="str">
+      <c r="D14" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E8_MODELO}}</v>
       </c>
-      <c r="E14" s="26" t="str">
+      <c r="E14" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E8_LAPIZ}}</v>
       </c>
-      <c r="F14" s="26" t="str">
+      <c r="F14" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E8_CUERDA}}</v>
       </c>
-      <c r="G14" s="26" t="str">
+      <c r="G14" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E8_CORREA}}</v>
       </c>
-      <c r="H14" s="26" t="str">
+      <c r="H14" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E8_TECLADO_NUM}}</v>
       </c>
-      <c r="I14" s="26" t="str">
+      <c r="I14" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E8_TECLADO_COMPL}}</v>
       </c>
-      <c r="J14" s="26" t="str">
+      <c r="J14" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E8_PANTALLA}}</v>
       </c>
-      <c r="K14" s="27" t="str">
+      <c r="K14" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E8_PROTECTOR}}</v>
       </c>
-      <c r="L14" s="26" t="str">
+      <c r="L14" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E8_BATERIA}}</v>
       </c>
-      <c r="M14" s="26" t="str">
+      <c r="M14" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E8_TAPA_BATERIA}}</v>
       </c>
-      <c r="N14" s="26" t="str">
+      <c r="N14" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E8_TARJETA_ALM}}</v>
       </c>
-      <c r="O14" s="26" t="str">
+      <c r="O14" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E8_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P14" s="26" t="str">
+      <c r="P14" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E8_CRISTAL}}</v>
       </c>
-      <c r="Q14" s="26" t="str">
+      <c r="Q14" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E8_CARCAZA_SUP}}</v>
       </c>
-      <c r="R14" s="26" t="str">
+      <c r="R14" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E8_CARCAZA_INF}}</v>
       </c>
-      <c r="S14" s="26" t="str">
+      <c r="S14" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E8_SIM}}</v>
       </c>
-      <c r="T14" s="49" t="str">
+      <c r="T14" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E8_PROBLEMA}}</v>
       </c>
-      <c r="U14" s="50"/>
-      <c r="V14" s="50"/>
-      <c r="W14" s="50"/>
-      <c r="X14" s="50"/>
-      <c r="Y14" s="50"/>
-      <c r="Z14" s="50"/>
-      <c r="AA14" s="51"/>
+      <c r="U14" s="33"/>
+      <c r="V14" s="33"/>
+      <c r="W14" s="33"/>
+      <c r="X14" s="33"/>
+      <c r="Y14" s="33"/>
+      <c r="Z14" s="33"/>
+      <c r="AA14" s="34"/>
       <c r="AB14" s="9"/>
       <c r="AC14" s="6"/>
     </row>
     <row r="15" spans="1:29" ht="138" customHeight="1">
-      <c r="A15" s="28">
+      <c r="A15" s="27">
         <v>9</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="30" t="str">
+      <c r="C15" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E9_SERIAL}}</v>
       </c>
-      <c r="D15" s="25" t="str">
+      <c r="D15" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E9_MODELO}}</v>
       </c>
-      <c r="E15" s="26" t="str">
+      <c r="E15" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E9_LAPIZ}}</v>
       </c>
-      <c r="F15" s="26" t="str">
+      <c r="F15" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E9_CUERDA}}</v>
       </c>
-      <c r="G15" s="26" t="str">
+      <c r="G15" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E9_CORREA}}</v>
       </c>
-      <c r="H15" s="26" t="str">
+      <c r="H15" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E9_TECLADO_NUM}}</v>
       </c>
-      <c r="I15" s="26" t="str">
+      <c r="I15" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E9_TECLADO_COMPL}}</v>
       </c>
-      <c r="J15" s="26" t="str">
+      <c r="J15" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E9_PANTALLA}}</v>
       </c>
-      <c r="K15" s="27" t="str">
+      <c r="K15" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E9_PROTECTOR}}</v>
       </c>
-      <c r="L15" s="26" t="str">
+      <c r="L15" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E9_BATERIA}}</v>
       </c>
-      <c r="M15" s="26" t="str">
+      <c r="M15" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E9_TAPA_BATERIA}}</v>
       </c>
-      <c r="N15" s="26" t="str">
+      <c r="N15" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E9_TARJETA_ALM}}</v>
       </c>
-      <c r="O15" s="26" t="str">
+      <c r="O15" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E9_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P15" s="26" t="str">
+      <c r="P15" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E9_CRISTAL}}</v>
       </c>
-      <c r="Q15" s="26" t="str">
+      <c r="Q15" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E9_CARCAZA_SUP}}</v>
       </c>
-      <c r="R15" s="26" t="str">
+      <c r="R15" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E9_CARCAZA_INF}}</v>
       </c>
-      <c r="S15" s="26" t="str">
+      <c r="S15" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E9_SIM}}</v>
       </c>
-      <c r="T15" s="49" t="str">
+      <c r="T15" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E9_PROBLEMA}}</v>
       </c>
-      <c r="U15" s="50"/>
-      <c r="V15" s="50"/>
-      <c r="W15" s="50"/>
-      <c r="X15" s="50"/>
-      <c r="Y15" s="50"/>
-      <c r="Z15" s="50"/>
-      <c r="AA15" s="51"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="33"/>
+      <c r="Z15" s="33"/>
+      <c r="AA15" s="34"/>
       <c r="AB15" s="9"/>
       <c r="AC15" s="6"/>
     </row>
     <row r="16" spans="1:29" ht="138" customHeight="1">
-      <c r="A16" s="28">
+      <c r="A16" s="27">
         <v>10</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="30" t="str">
+      <c r="C16" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E10_SERIAL}}</v>
       </c>
-      <c r="D16" s="25" t="str">
+      <c r="D16" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E10_MODELO}}</v>
       </c>
-      <c r="E16" s="26" t="str">
+      <c r="E16" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E10_LAPIZ}}</v>
       </c>
-      <c r="F16" s="26" t="str">
+      <c r="F16" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E10_CUERDA}}</v>
       </c>
-      <c r="G16" s="26" t="str">
+      <c r="G16" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E10_CORREA}}</v>
       </c>
-      <c r="H16" s="26" t="str">
+      <c r="H16" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E10_TECLADO_NUM}}</v>
       </c>
-      <c r="I16" s="26" t="str">
+      <c r="I16" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E10_TECLADO_COMPL}}</v>
       </c>
-      <c r="J16" s="26" t="str">
+      <c r="J16" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E10_PANTALLA}}</v>
       </c>
-      <c r="K16" s="27" t="str">
+      <c r="K16" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E10_PROTECTOR}}</v>
       </c>
-      <c r="L16" s="26" t="str">
+      <c r="L16" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E10_BATERIA}}</v>
       </c>
-      <c r="M16" s="26" t="str">
+      <c r="M16" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E10_TAPA_BATERIA}}</v>
       </c>
-      <c r="N16" s="26" t="str">
+      <c r="N16" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E10_TARJETA_ALM}}</v>
       </c>
-      <c r="O16" s="26" t="str">
+      <c r="O16" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E10_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P16" s="26" t="str">
+      <c r="P16" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E10_CRISTAL}}</v>
       </c>
-      <c r="Q16" s="26" t="str">
+      <c r="Q16" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E10_CARCAZA_SUP}}</v>
       </c>
-      <c r="R16" s="26" t="str">
+      <c r="R16" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E10_CARCAZA_INF}}</v>
       </c>
-      <c r="S16" s="26" t="str">
+      <c r="S16" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E10_SIM}}</v>
       </c>
-      <c r="T16" s="49" t="str">
+      <c r="T16" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E10_PROBLEMA}}</v>
       </c>
-      <c r="U16" s="50"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="50"/>
-      <c r="X16" s="50"/>
-      <c r="Y16" s="50"/>
-      <c r="Z16" s="50"/>
-      <c r="AA16" s="51"/>
+      <c r="U16" s="33"/>
+      <c r="V16" s="33"/>
+      <c r="W16" s="33"/>
+      <c r="X16" s="33"/>
+      <c r="Y16" s="33"/>
+      <c r="Z16" s="33"/>
+      <c r="AA16" s="34"/>
       <c r="AB16" s="9"/>
       <c r="AC16" s="6"/>
     </row>
     <row r="17" spans="1:29" ht="138" customHeight="1">
-      <c r="A17" s="28">
+      <c r="A17" s="27">
         <v>11</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="30" t="str">
+      <c r="C17" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E11_SERIAL}}</v>
       </c>
-      <c r="D17" s="25" t="str">
+      <c r="D17" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E11_MODELO}}</v>
       </c>
-      <c r="E17" s="26" t="str">
+      <c r="E17" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E11_LAPIZ}}</v>
       </c>
-      <c r="F17" s="26" t="str">
+      <c r="F17" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E11_CUERDA}}</v>
       </c>
-      <c r="G17" s="26" t="str">
+      <c r="G17" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E11_CORREA}}</v>
       </c>
-      <c r="H17" s="26" t="str">
+      <c r="H17" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E11_TECLADO_NUM}}</v>
       </c>
-      <c r="I17" s="26" t="str">
+      <c r="I17" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E11_TECLADO_COMPL}}</v>
       </c>
-      <c r="J17" s="26" t="str">
+      <c r="J17" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E11_PANTALLA}}</v>
       </c>
-      <c r="K17" s="27" t="str">
+      <c r="K17" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E11_PROTECTOR}}</v>
       </c>
-      <c r="L17" s="26" t="str">
+      <c r="L17" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E11_BATERIA}}</v>
       </c>
-      <c r="M17" s="26" t="str">
+      <c r="M17" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E11_TAPA_BATERIA}}</v>
       </c>
-      <c r="N17" s="26" t="str">
+      <c r="N17" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E11_TARJETA_ALM}}</v>
       </c>
-      <c r="O17" s="26" t="str">
+      <c r="O17" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E11_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P17" s="26" t="str">
+      <c r="P17" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E11_CRISTAL}}</v>
       </c>
-      <c r="Q17" s="26" t="str">
+      <c r="Q17" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E11_CARCAZA_SUP}}</v>
       </c>
-      <c r="R17" s="26" t="str">
+      <c r="R17" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E11_CARCAZA_INF}}</v>
       </c>
-      <c r="S17" s="26" t="str">
+      <c r="S17" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E11_SIM}}</v>
       </c>
-      <c r="T17" s="49" t="str">
+      <c r="T17" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E11_PROBLEMA}}</v>
       </c>
-      <c r="U17" s="50"/>
-      <c r="V17" s="50"/>
-      <c r="W17" s="50"/>
-      <c r="X17" s="50"/>
-      <c r="Y17" s="50"/>
-      <c r="Z17" s="50"/>
-      <c r="AA17" s="51"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="33"/>
+      <c r="X17" s="33"/>
+      <c r="Y17" s="33"/>
+      <c r="Z17" s="33"/>
+      <c r="AA17" s="34"/>
       <c r="AB17" s="9"/>
       <c r="AC17" s="6"/>
     </row>
     <row r="18" spans="1:29" ht="138" customHeight="1">
-      <c r="A18" s="28">
+      <c r="A18" s="27">
         <v>12</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="30" t="str">
+      <c r="C18" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E12_SERIAL}}</v>
       </c>
-      <c r="D18" s="25" t="str">
+      <c r="D18" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E12_MODELO}}</v>
       </c>
-      <c r="E18" s="26" t="str">
+      <c r="E18" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E12_LAPIZ}}</v>
       </c>
-      <c r="F18" s="26" t="str">
+      <c r="F18" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E12_CUERDA}}</v>
       </c>
-      <c r="G18" s="26" t="str">
+      <c r="G18" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E12_CORREA}}</v>
       </c>
-      <c r="H18" s="26" t="str">
+      <c r="H18" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E12_TECLADO_NUM}}</v>
       </c>
-      <c r="I18" s="26" t="str">
+      <c r="I18" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E12_TECLADO_COMPL}}</v>
       </c>
-      <c r="J18" s="26" t="str">
+      <c r="J18" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E12_PANTALLA}}</v>
       </c>
-      <c r="K18" s="27" t="str">
+      <c r="K18" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E12_PROTECTOR}}</v>
       </c>
-      <c r="L18" s="26" t="str">
+      <c r="L18" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E12_BATERIA}}</v>
       </c>
-      <c r="M18" s="26" t="str">
+      <c r="M18" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E12_TAPA_BATERIA}}</v>
       </c>
-      <c r="N18" s="26" t="str">
+      <c r="N18" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E12_TARJETA_ALM}}</v>
       </c>
-      <c r="O18" s="26" t="str">
+      <c r="O18" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E12_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P18" s="26" t="str">
+      <c r="P18" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E12_CRISTAL}}</v>
       </c>
-      <c r="Q18" s="26" t="str">
+      <c r="Q18" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E12_CARCAZA_SUP}}</v>
       </c>
-      <c r="R18" s="26" t="str">
+      <c r="R18" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E12_CARCAZA_INF}}</v>
       </c>
-      <c r="S18" s="26" t="str">
+      <c r="S18" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E12_SIM}}</v>
       </c>
-      <c r="T18" s="49" t="str">
+      <c r="T18" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E12_PROBLEMA}}</v>
       </c>
-      <c r="U18" s="50"/>
-      <c r="V18" s="50"/>
-      <c r="W18" s="50"/>
-      <c r="X18" s="50"/>
-      <c r="Y18" s="50"/>
-      <c r="Z18" s="50"/>
-      <c r="AA18" s="51"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="33"/>
+      <c r="Y18" s="33"/>
+      <c r="Z18" s="33"/>
+      <c r="AA18" s="34"/>
       <c r="AB18" s="9"/>
       <c r="AC18" s="6"/>
     </row>
     <row r="19" spans="1:29" ht="138" customHeight="1">
-      <c r="A19" s="28">
+      <c r="A19" s="27">
         <v>13</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="30" t="str">
+      <c r="C19" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E13_SERIAL}}</v>
       </c>
-      <c r="D19" s="25" t="str">
+      <c r="D19" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E13_MODELO}}</v>
       </c>
-      <c r="E19" s="26" t="str">
+      <c r="E19" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E13_LAPIZ}}</v>
       </c>
-      <c r="F19" s="26" t="str">
+      <c r="F19" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E13_CUERDA}}</v>
       </c>
-      <c r="G19" s="26" t="str">
+      <c r="G19" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E13_CORREA}}</v>
       </c>
-      <c r="H19" s="26" t="str">
+      <c r="H19" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E13_TECLADO_NUM}}</v>
       </c>
-      <c r="I19" s="26" t="str">
+      <c r="I19" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E13_TECLADO_COMPL}}</v>
       </c>
-      <c r="J19" s="26" t="str">
+      <c r="J19" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E13_PANTALLA}}</v>
       </c>
-      <c r="K19" s="27" t="str">
+      <c r="K19" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E13_PROTECTOR}}</v>
       </c>
-      <c r="L19" s="26" t="str">
+      <c r="L19" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E13_BATERIA}}</v>
       </c>
-      <c r="M19" s="26" t="str">
+      <c r="M19" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E13_TAPA_BATERIA}}</v>
       </c>
-      <c r="N19" s="26" t="str">
+      <c r="N19" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E13_TARJETA_ALM}}</v>
       </c>
-      <c r="O19" s="26" t="str">
+      <c r="O19" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E13_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P19" s="26" t="str">
+      <c r="P19" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E13_CRISTAL}}</v>
       </c>
-      <c r="Q19" s="26" t="str">
+      <c r="Q19" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E13_CARCAZA_SUP}}</v>
       </c>
-      <c r="R19" s="26" t="str">
+      <c r="R19" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E13_CARCAZA_INF}}</v>
       </c>
-      <c r="S19" s="26" t="str">
+      <c r="S19" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E13_SIM}}</v>
       </c>
-      <c r="T19" s="49" t="str">
+      <c r="T19" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E13_PROBLEMA}}</v>
       </c>
-      <c r="U19" s="50"/>
-      <c r="V19" s="50"/>
-      <c r="W19" s="50"/>
-      <c r="X19" s="50"/>
-      <c r="Y19" s="50"/>
-      <c r="Z19" s="50"/>
-      <c r="AA19" s="51"/>
+      <c r="U19" s="33"/>
+      <c r="V19" s="33"/>
+      <c r="W19" s="33"/>
+      <c r="X19" s="33"/>
+      <c r="Y19" s="33"/>
+      <c r="Z19" s="33"/>
+      <c r="AA19" s="34"/>
       <c r="AB19" s="9"/>
       <c r="AC19" s="6"/>
     </row>
     <row r="20" spans="1:29" ht="138" customHeight="1">
-      <c r="A20" s="28">
+      <c r="A20" s="27">
         <v>14</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="30" t="str">
+      <c r="C20" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E14_SERIAL}}</v>
       </c>
-      <c r="D20" s="25" t="str">
+      <c r="D20" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E14_MODELO}}</v>
       </c>
-      <c r="E20" s="26" t="str">
+      <c r="E20" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E14_LAPIZ}}</v>
       </c>
-      <c r="F20" s="26" t="str">
+      <c r="F20" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E14_CUERDA}}</v>
       </c>
-      <c r="G20" s="26" t="str">
+      <c r="G20" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E14_CORREA}}</v>
       </c>
-      <c r="H20" s="26" t="str">
+      <c r="H20" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E14_TECLADO_NUM}}</v>
       </c>
-      <c r="I20" s="26" t="str">
+      <c r="I20" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E14_TECLADO_COMPL}}</v>
       </c>
-      <c r="J20" s="26" t="str">
+      <c r="J20" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E14_PANTALLA}}</v>
       </c>
-      <c r="K20" s="27" t="str">
+      <c r="K20" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E14_PROTECTOR}}</v>
       </c>
-      <c r="L20" s="26" t="str">
+      <c r="L20" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E14_BATERIA}}</v>
       </c>
-      <c r="M20" s="26" t="str">
+      <c r="M20" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E14_TAPA_BATERIA}}</v>
       </c>
-      <c r="N20" s="26" t="str">
+      <c r="N20" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E14_TARJETA_ALM}}</v>
       </c>
-      <c r="O20" s="26" t="str">
+      <c r="O20" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E14_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P20" s="26" t="str">
+      <c r="P20" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E14_CRISTAL}}</v>
       </c>
-      <c r="Q20" s="26" t="str">
+      <c r="Q20" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E14_CARCAZA_SUP}}</v>
       </c>
-      <c r="R20" s="26" t="str">
+      <c r="R20" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E14_CARCAZA_INF}}</v>
       </c>
-      <c r="S20" s="26" t="str">
+      <c r="S20" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E14_SIM}}</v>
       </c>
-      <c r="T20" s="49" t="str">
+      <c r="T20" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E14_PROBLEMA}}</v>
       </c>
-      <c r="U20" s="50"/>
-      <c r="V20" s="50"/>
-      <c r="W20" s="50"/>
-      <c r="X20" s="50"/>
-      <c r="Y20" s="50"/>
-      <c r="Z20" s="50"/>
-      <c r="AA20" s="51"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="33"/>
+      <c r="X20" s="33"/>
+      <c r="Y20" s="33"/>
+      <c r="Z20" s="33"/>
+      <c r="AA20" s="34"/>
       <c r="AB20" s="9"/>
       <c r="AC20" s="6"/>
     </row>
     <row r="21" spans="1:29" ht="138" customHeight="1">
-      <c r="A21" s="28">
+      <c r="A21" s="27">
         <v>15</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="30" t="str">
+      <c r="C21" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E15_SERIAL}}</v>
       </c>
-      <c r="D21" s="25" t="str">
+      <c r="D21" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E15_MODELO}}</v>
       </c>
-      <c r="E21" s="26" t="str">
+      <c r="E21" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E15_LAPIZ}}</v>
       </c>
-      <c r="F21" s="26" t="str">
+      <c r="F21" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E15_CUERDA}}</v>
       </c>
-      <c r="G21" s="26" t="str">
+      <c r="G21" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E15_CORREA}}</v>
       </c>
-      <c r="H21" s="26" t="str">
+      <c r="H21" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E15_TECLADO_NUM}}</v>
       </c>
-      <c r="I21" s="26" t="str">
+      <c r="I21" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E15_TECLADO_COMPL}}</v>
       </c>
-      <c r="J21" s="26" t="str">
+      <c r="J21" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E15_PANTALLA}}</v>
       </c>
-      <c r="K21" s="27" t="str">
+      <c r="K21" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E15_PROTECTOR}}</v>
       </c>
-      <c r="L21" s="26" t="str">
+      <c r="L21" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E15_BATERIA}}</v>
       </c>
-      <c r="M21" s="26" t="str">
+      <c r="M21" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E15_TAPA_BATERIA}}</v>
       </c>
-      <c r="N21" s="26" t="str">
+      <c r="N21" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E15_TARJETA_ALM}}</v>
       </c>
-      <c r="O21" s="26" t="str">
+      <c r="O21" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E15_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P21" s="26" t="str">
+      <c r="P21" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E15_CRISTAL}}</v>
       </c>
-      <c r="Q21" s="26" t="str">
+      <c r="Q21" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E15_CARCAZA_SUP}}</v>
       </c>
-      <c r="R21" s="26" t="str">
+      <c r="R21" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E15_CARCAZA_INF}}</v>
       </c>
-      <c r="S21" s="26" t="str">
+      <c r="S21" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E15_SIM}}</v>
       </c>
-      <c r="T21" s="49" t="str">
+      <c r="T21" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E15_PROBLEMA}}</v>
       </c>
-      <c r="U21" s="50"/>
-      <c r="V21" s="50"/>
-      <c r="W21" s="50"/>
-      <c r="X21" s="50"/>
-      <c r="Y21" s="50"/>
-      <c r="Z21" s="50"/>
-      <c r="AA21" s="51"/>
+      <c r="U21" s="33"/>
+      <c r="V21" s="33"/>
+      <c r="W21" s="33"/>
+      <c r="X21" s="33"/>
+      <c r="Y21" s="33"/>
+      <c r="Z21" s="33"/>
+      <c r="AA21" s="34"/>
       <c r="AB21" s="9"/>
       <c r="AC21" s="6"/>
     </row>
     <row r="22" spans="1:29" ht="138" customHeight="1">
-      <c r="A22" s="28">
+      <c r="A22" s="27">
         <v>16</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="30" t="str">
+      <c r="C22" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E16_SERIAL}}</v>
       </c>
-      <c r="D22" s="25" t="str">
+      <c r="D22" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E16_MODELO}}</v>
       </c>
-      <c r="E22" s="26" t="str">
+      <c r="E22" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E16_LAPIZ}}</v>
       </c>
-      <c r="F22" s="26" t="str">
+      <c r="F22" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E16_CUERDA}}</v>
       </c>
-      <c r="G22" s="26" t="str">
+      <c r="G22" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E16_CORREA}}</v>
       </c>
-      <c r="H22" s="26" t="str">
+      <c r="H22" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E16_TECLADO_NUM}}</v>
       </c>
-      <c r="I22" s="26" t="str">
+      <c r="I22" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E16_TECLADO_COMPL}}</v>
       </c>
-      <c r="J22" s="26" t="str">
+      <c r="J22" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E16_PANTALLA}}</v>
       </c>
-      <c r="K22" s="27" t="str">
+      <c r="K22" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E16_PROTECTOR}}</v>
       </c>
-      <c r="L22" s="26" t="str">
+      <c r="L22" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E16_BATERIA}}</v>
       </c>
-      <c r="M22" s="26" t="str">
+      <c r="M22" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E16_TAPA_BATERIA}}</v>
       </c>
-      <c r="N22" s="26" t="str">
+      <c r="N22" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E16_TARJETA_ALM}}</v>
       </c>
-      <c r="O22" s="26" t="str">
+      <c r="O22" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E16_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P22" s="26" t="str">
+      <c r="P22" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E16_CRISTAL}}</v>
       </c>
-      <c r="Q22" s="26" t="str">
+      <c r="Q22" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E16_CARCAZA_SUP}}</v>
       </c>
-      <c r="R22" s="26" t="str">
+      <c r="R22" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E16_CARCAZA_INF}}</v>
       </c>
-      <c r="S22" s="26" t="str">
+      <c r="S22" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E16_SIM}}</v>
       </c>
-      <c r="T22" s="49" t="str">
+      <c r="T22" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E16_PROBLEMA}}</v>
       </c>
-      <c r="U22" s="50"/>
-      <c r="V22" s="50"/>
-      <c r="W22" s="50"/>
-      <c r="X22" s="50"/>
-      <c r="Y22" s="50"/>
-      <c r="Z22" s="50"/>
-      <c r="AA22" s="51"/>
+      <c r="U22" s="33"/>
+      <c r="V22" s="33"/>
+      <c r="W22" s="33"/>
+      <c r="X22" s="33"/>
+      <c r="Y22" s="33"/>
+      <c r="Z22" s="33"/>
+      <c r="AA22" s="34"/>
       <c r="AB22" s="9"/>
       <c r="AC22" s="6"/>
     </row>
     <row r="23" spans="1:29" ht="138" customHeight="1">
-      <c r="A23" s="28">
+      <c r="A23" s="27">
         <v>17</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="30" t="str">
+      <c r="C23" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E17_SERIAL}}</v>
       </c>
-      <c r="D23" s="25" t="str">
+      <c r="D23" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E17_MODELO}}</v>
       </c>
-      <c r="E23" s="26" t="str">
+      <c r="E23" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E17_LAPIZ}}</v>
       </c>
-      <c r="F23" s="26" t="str">
+      <c r="F23" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E17_CUERDA}}</v>
       </c>
-      <c r="G23" s="26" t="str">
+      <c r="G23" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E17_CORREA}}</v>
       </c>
-      <c r="H23" s="26" t="str">
+      <c r="H23" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E17_TECLADO_NUM}}</v>
       </c>
-      <c r="I23" s="26" t="str">
+      <c r="I23" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E17_TECLADO_COMPL}}</v>
       </c>
-      <c r="J23" s="26" t="str">
+      <c r="J23" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E17_PANTALLA}}</v>
       </c>
-      <c r="K23" s="27" t="str">
+      <c r="K23" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E17_PROTECTOR}}</v>
       </c>
-      <c r="L23" s="26" t="str">
+      <c r="L23" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E17_BATERIA}}</v>
       </c>
-      <c r="M23" s="26" t="str">
+      <c r="M23" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E17_TAPA_BATERIA}}</v>
       </c>
-      <c r="N23" s="26" t="str">
+      <c r="N23" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E17_TARJETA_ALM}}</v>
       </c>
-      <c r="O23" s="26" t="str">
+      <c r="O23" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E17_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P23" s="26" t="str">
+      <c r="P23" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E17_CRISTAL}}</v>
       </c>
-      <c r="Q23" s="26" t="str">
+      <c r="Q23" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E17_CARCAZA_SUP}}</v>
       </c>
-      <c r="R23" s="26" t="str">
+      <c r="R23" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E17_CARCAZA_INF}}</v>
       </c>
-      <c r="S23" s="26" t="str">
+      <c r="S23" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E17_SIM}}</v>
       </c>
-      <c r="T23" s="49" t="str">
+      <c r="T23" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E17_PROBLEMA}}</v>
       </c>
-      <c r="U23" s="50"/>
-      <c r="V23" s="50"/>
-      <c r="W23" s="50"/>
-      <c r="X23" s="50"/>
-      <c r="Y23" s="50"/>
-      <c r="Z23" s="50"/>
-      <c r="AA23" s="51"/>
+      <c r="U23" s="33"/>
+      <c r="V23" s="33"/>
+      <c r="W23" s="33"/>
+      <c r="X23" s="33"/>
+      <c r="Y23" s="33"/>
+      <c r="Z23" s="33"/>
+      <c r="AA23" s="34"/>
       <c r="AB23" s="9"/>
       <c r="AC23" s="6"/>
     </row>
     <row r="24" spans="1:29" ht="138" customHeight="1">
-      <c r="A24" s="28">
+      <c r="A24" s="27">
         <v>18</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="30" t="str">
+      <c r="C24" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E18_SERIAL}}</v>
       </c>
-      <c r="D24" s="25" t="str">
+      <c r="D24" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E18_MODELO}}</v>
       </c>
-      <c r="E24" s="26" t="str">
+      <c r="E24" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E18_LAPIZ}}</v>
       </c>
-      <c r="F24" s="26" t="str">
+      <c r="F24" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E18_CUERDA}}</v>
       </c>
-      <c r="G24" s="26" t="str">
+      <c r="G24" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E18_CORREA}}</v>
       </c>
-      <c r="H24" s="26" t="str">
+      <c r="H24" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E18_TECLADO_NUM}}</v>
       </c>
-      <c r="I24" s="26" t="str">
+      <c r="I24" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E18_TECLADO_COMPL}}</v>
       </c>
-      <c r="J24" s="26" t="str">
+      <c r="J24" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E18_PANTALLA}}</v>
       </c>
-      <c r="K24" s="27" t="str">
+      <c r="K24" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E18_PROTECTOR}}</v>
       </c>
-      <c r="L24" s="26" t="str">
+      <c r="L24" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E18_BATERIA}}</v>
       </c>
-      <c r="M24" s="26" t="str">
+      <c r="M24" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E18_TAPA_BATERIA}}</v>
       </c>
-      <c r="N24" s="26" t="str">
+      <c r="N24" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E18_TARJETA_ALM}}</v>
       </c>
-      <c r="O24" s="26" t="str">
+      <c r="O24" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E18_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P24" s="26" t="str">
+      <c r="P24" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E18_CRISTAL}}</v>
       </c>
-      <c r="Q24" s="26" t="str">
+      <c r="Q24" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E18_CARCAZA_SUP}}</v>
       </c>
-      <c r="R24" s="26" t="str">
+      <c r="R24" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E18_CARCAZA_INF}}</v>
       </c>
-      <c r="S24" s="26" t="str">
+      <c r="S24" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E18_SIM}}</v>
       </c>
-      <c r="T24" s="49" t="str">
+      <c r="T24" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E18_PROBLEMA}}</v>
       </c>
-      <c r="U24" s="50"/>
-      <c r="V24" s="50"/>
-      <c r="W24" s="50"/>
-      <c r="X24" s="50"/>
-      <c r="Y24" s="50"/>
-      <c r="Z24" s="50"/>
-      <c r="AA24" s="51"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="33"/>
+      <c r="X24" s="33"/>
+      <c r="Y24" s="33"/>
+      <c r="Z24" s="33"/>
+      <c r="AA24" s="34"/>
       <c r="AB24" s="9"/>
       <c r="AC24" s="6"/>
     </row>
     <row r="25" spans="1:29" ht="138" customHeight="1">
-      <c r="A25" s="28">
+      <c r="A25" s="27">
         <v>19</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="30" t="str">
+      <c r="C25" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E19_SERIAL}}</v>
       </c>
-      <c r="D25" s="25" t="str">
+      <c r="D25" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E19_MODELO}}</v>
       </c>
-      <c r="E25" s="26" t="str">
+      <c r="E25" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E19_LAPIZ}}</v>
       </c>
-      <c r="F25" s="26" t="str">
+      <c r="F25" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E19_CUERDA}}</v>
       </c>
-      <c r="G25" s="26" t="str">
+      <c r="G25" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E19_CORREA}}</v>
       </c>
-      <c r="H25" s="26" t="str">
+      <c r="H25" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E19_TECLADO_NUM}}</v>
       </c>
-      <c r="I25" s="26" t="str">
+      <c r="I25" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E19_TECLADO_COMPL}}</v>
       </c>
-      <c r="J25" s="26" t="str">
+      <c r="J25" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E19_PANTALLA}}</v>
       </c>
-      <c r="K25" s="27" t="str">
+      <c r="K25" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E19_PROTECTOR}}</v>
       </c>
-      <c r="L25" s="26" t="str">
+      <c r="L25" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E19_BATERIA}}</v>
       </c>
-      <c r="M25" s="26" t="str">
+      <c r="M25" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E19_TAPA_BATERIA}}</v>
       </c>
-      <c r="N25" s="26" t="str">
+      <c r="N25" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E19_TARJETA_ALM}}</v>
       </c>
-      <c r="O25" s="26" t="str">
+      <c r="O25" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E19_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P25" s="26" t="str">
+      <c r="P25" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E19_CRISTAL}}</v>
       </c>
-      <c r="Q25" s="26" t="str">
+      <c r="Q25" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E19_CARCAZA_SUP}}</v>
       </c>
-      <c r="R25" s="26" t="str">
+      <c r="R25" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E19_CARCAZA_INF}}</v>
       </c>
-      <c r="S25" s="26" t="str">
+      <c r="S25" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E19_SIM}}</v>
       </c>
-      <c r="T25" s="49" t="str">
+      <c r="T25" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E19_PROBLEMA}}</v>
       </c>
-      <c r="U25" s="50"/>
-      <c r="V25" s="50"/>
-      <c r="W25" s="50"/>
-      <c r="X25" s="50"/>
-      <c r="Y25" s="50"/>
-      <c r="Z25" s="50"/>
-      <c r="AA25" s="51"/>
+      <c r="U25" s="33"/>
+      <c r="V25" s="33"/>
+      <c r="W25" s="33"/>
+      <c r="X25" s="33"/>
+      <c r="Y25" s="33"/>
+      <c r="Z25" s="33"/>
+      <c r="AA25" s="34"/>
       <c r="AB25" s="9"/>
       <c r="AC25" s="6"/>
     </row>
     <row r="26" spans="1:29" ht="138" customHeight="1">
-      <c r="A26" s="29">
+      <c r="A26" s="28">
         <v>20</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="30" t="str">
+      <c r="C26" s="29" t="str">
         <f t="shared" si="0"/>
         <v>{{E20_SERIAL}}</v>
       </c>
-      <c r="D26" s="25" t="str">
+      <c r="D26" s="24" t="str">
         <f t="shared" si="1"/>
         <v>{{E20_MODELO}}</v>
       </c>
-      <c r="E26" s="26" t="str">
+      <c r="E26" s="25" t="str">
         <f t="shared" si="2"/>
         <v>{{E20_LAPIZ}}</v>
       </c>
-      <c r="F26" s="26" t="str">
+      <c r="F26" s="25" t="str">
         <f t="shared" si="3"/>
         <v>{{E20_CUERDA}}</v>
       </c>
-      <c r="G26" s="26" t="str">
+      <c r="G26" s="25" t="str">
         <f t="shared" si="4"/>
         <v>{{E20_CORREA}}</v>
       </c>
-      <c r="H26" s="26" t="str">
+      <c r="H26" s="25" t="str">
         <f t="shared" si="5"/>
         <v>{{E20_TECLADO_NUM}}</v>
       </c>
-      <c r="I26" s="26" t="str">
+      <c r="I26" s="25" t="str">
         <f t="shared" si="6"/>
         <v>{{E20_TECLADO_COMPL}}</v>
       </c>
-      <c r="J26" s="26" t="str">
+      <c r="J26" s="25" t="str">
         <f t="shared" si="7"/>
         <v>{{E20_PANTALLA}}</v>
       </c>
-      <c r="K26" s="27" t="str">
+      <c r="K26" s="26" t="str">
         <f t="shared" si="8"/>
         <v>{{E20_PROTECTOR}}</v>
       </c>
-      <c r="L26" s="26" t="str">
+      <c r="L26" s="25" t="str">
         <f t="shared" si="9"/>
         <v>{{E20_BATERIA}}</v>
       </c>
-      <c r="M26" s="26" t="str">
+      <c r="M26" s="25" t="str">
         <f t="shared" si="10"/>
         <v>{{E20_TAPA_BATERIA}}</v>
       </c>
-      <c r="N26" s="26" t="str">
+      <c r="N26" s="25" t="str">
         <f t="shared" si="11"/>
         <v>{{E20_TARJETA_ALM}}</v>
       </c>
-      <c r="O26" s="26" t="str">
+      <c r="O26" s="25" t="str">
         <f t="shared" si="12"/>
         <v>{{E20_CUBIERTA_TARJETA}}</v>
       </c>
-      <c r="P26" s="26" t="str">
+      <c r="P26" s="25" t="str">
         <f t="shared" si="13"/>
         <v>{{E20_CRISTAL}}</v>
       </c>
-      <c r="Q26" s="26" t="str">
+      <c r="Q26" s="25" t="str">
         <f t="shared" si="14"/>
         <v>{{E20_CARCAZA_SUP}}</v>
       </c>
-      <c r="R26" s="26" t="str">
+      <c r="R26" s="25" t="str">
         <f t="shared" si="15"/>
         <v>{{E20_CARCAZA_INF}}</v>
       </c>
-      <c r="S26" s="26" t="str">
+      <c r="S26" s="25" t="str">
         <f t="shared" si="16"/>
         <v>{{E20_SIM}}</v>
       </c>
-      <c r="T26" s="49" t="str">
+      <c r="T26" s="32" t="str">
         <f t="shared" si="17"/>
         <v>{{E20_PROBLEMA}}</v>
       </c>
-      <c r="U26" s="50"/>
-      <c r="V26" s="50"/>
-      <c r="W26" s="50"/>
-      <c r="X26" s="50"/>
-      <c r="Y26" s="50"/>
-      <c r="Z26" s="50"/>
-      <c r="AA26" s="51"/>
+      <c r="U26" s="33"/>
+      <c r="V26" s="33"/>
+      <c r="W26" s="33"/>
+      <c r="X26" s="33"/>
+      <c r="Y26" s="33"/>
+      <c r="Z26" s="33"/>
+      <c r="AA26" s="34"/>
       <c r="AB26" s="9"/>
       <c r="AC26" s="6"/>
     </row>
     <row r="27" spans="1:29" ht="25.5" customHeight="1">
-      <c r="B27" s="31"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -3189,63 +3191,63 @@
       <c r="AA27" s="10"/>
     </row>
     <row r="28" spans="1:29" ht="59.25" customHeight="1">
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
-      <c r="N28" s="36"/>
-      <c r="O28" s="36"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="36"/>
-      <c r="R28" s="36"/>
-      <c r="S28" s="36"/>
-      <c r="T28" s="36"/>
-      <c r="U28" s="36"/>
-      <c r="V28" s="36"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="51"/>
+      <c r="R28" s="51"/>
+      <c r="S28" s="51"/>
+      <c r="T28" s="51"/>
+      <c r="U28" s="51"/>
+      <c r="V28" s="51"/>
       <c r="W28" s="11"/>
-      <c r="X28" s="37" t="s">
+      <c r="X28" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="Y28" s="37"/>
+      <c r="Y28" s="52"/>
       <c r="Z28" s="12" t="s">
         <v>29</v>
       </c>
       <c r="AA28" s="13"/>
     </row>
     <row r="29" spans="1:29" ht="69.75" customHeight="1">
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
-      <c r="O29" s="38"/>
-      <c r="P29" s="38"/>
-      <c r="Q29" s="38"/>
-      <c r="R29" s="38"/>
-      <c r="S29" s="38"/>
-      <c r="T29" s="38"/>
-      <c r="U29" s="38"/>
-      <c r="V29" s="38"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="53"/>
+      <c r="S29" s="53"/>
+      <c r="T29" s="53"/>
+      <c r="U29" s="53"/>
+      <c r="V29" s="53"/>
       <c r="W29" s="11"/>
       <c r="X29" s="14"/>
       <c r="Y29" s="14"/>
@@ -3325,34 +3327,34 @@
       <c r="R32" s="17"/>
     </row>
     <row r="33" spans="1:27" ht="31.5" customHeight="1">
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
       <c r="E33" s="17"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
       <c r="P33" s="17"/>
-      <c r="Q33" s="52" t="s">
+      <c r="Q33" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="R33" s="52"/>
-      <c r="S33" s="52"/>
-      <c r="T33" s="52"/>
-      <c r="U33" s="52"/>
-      <c r="V33" s="52"/>
-      <c r="W33" s="52"/>
-      <c r="X33" s="52"/>
-      <c r="Y33" s="52"/>
-      <c r="Z33" s="52"/>
-      <c r="AA33" s="52"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="35"/>
+      <c r="U33" s="35"/>
+      <c r="V33" s="35"/>
+      <c r="W33" s="35"/>
+      <c r="X33" s="35"/>
+      <c r="Y33" s="35"/>
+      <c r="Z33" s="35"/>
+      <c r="AA33" s="35"/>
     </row>
     <row r="34" spans="1:27" ht="23.25" customHeight="1">
       <c r="B34" s="16" t="s">
@@ -3378,22 +3380,24 @@
       <c r="R34" s="17"/>
     </row>
     <row r="35" spans="1:27" ht="31.5" customHeight="1">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
       <c r="E35" s="17"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="39"/>
+      <c r="F35" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="37"/>
       <c r="P35" s="20"/>
       <c r="Q35" s="19"/>
       <c r="R35" s="18"/>
@@ -3431,22 +3435,24 @@
       <c r="R36" s="17"/>
     </row>
     <row r="37" spans="1:27" ht="23.25" customHeight="1">
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
       <c r="E37" s="17"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="22"/>
+      <c r="F37" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="38"/>
       <c r="P37" s="17"/>
       <c r="Q37" s="18"/>
       <c r="R37" s="18"/>
@@ -3484,112 +3490,96 @@
       <c r="R38" s="17"/>
     </row>
     <row r="39" spans="1:27" ht="18.75" customHeight="1">
-      <c r="B39" s="24"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="23"/>
-      <c r="P39" s="23"/>
-      <c r="Q39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="22"/>
+      <c r="P39" s="22"/>
+      <c r="Q39" s="22"/>
     </row>
     <row r="40" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="34"/>
-      <c r="N40" s="35" t="s">
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="40"/>
+      <c r="N40" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="R40" s="35"/>
-      <c r="S40" s="35"/>
-      <c r="T40" s="35"/>
-      <c r="U40" s="35"/>
-      <c r="V40" s="35"/>
-      <c r="W40" s="35"/>
-      <c r="X40" s="35"/>
-      <c r="Y40" s="35"/>
-      <c r="Z40" s="35"/>
-      <c r="AA40" s="35"/>
+      <c r="O40" s="50"/>
+      <c r="P40" s="50"/>
+      <c r="Q40" s="50"/>
+      <c r="R40" s="50"/>
+      <c r="S40" s="50"/>
+      <c r="T40" s="50"/>
+      <c r="U40" s="50"/>
+      <c r="V40" s="50"/>
+      <c r="W40" s="50"/>
+      <c r="X40" s="50"/>
+      <c r="Y40" s="50"/>
+      <c r="Z40" s="50"/>
+      <c r="AA40" s="50"/>
     </row>
     <row r="41" spans="1:27" ht="87.75" customHeight="1">
-      <c r="A41" s="33"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="34"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
-      <c r="S41" s="35"/>
-      <c r="T41" s="35"/>
-      <c r="U41" s="35"/>
-      <c r="V41" s="35"/>
-      <c r="W41" s="35"/>
-      <c r="X41" s="35"/>
-      <c r="Y41" s="35"/>
-      <c r="Z41" s="35"/>
-      <c r="AA41" s="35"/>
+      <c r="A41" s="49"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="40"/>
+      <c r="N41" s="50"/>
+      <c r="O41" s="50"/>
+      <c r="P41" s="50"/>
+      <c r="Q41" s="50"/>
+      <c r="R41" s="50"/>
+      <c r="S41" s="50"/>
+      <c r="T41" s="50"/>
+      <c r="U41" s="50"/>
+      <c r="V41" s="50"/>
+      <c r="W41" s="50"/>
+      <c r="X41" s="50"/>
+      <c r="Y41" s="50"/>
+      <c r="Z41" s="50"/>
+      <c r="AA41" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="T22:AA22"/>
-    <mergeCell ref="T23:AA23"/>
-    <mergeCell ref="T24:AA24"/>
-    <mergeCell ref="T25:AA25"/>
-    <mergeCell ref="T17:AA17"/>
-    <mergeCell ref="T18:AA18"/>
-    <mergeCell ref="T19:AA19"/>
-    <mergeCell ref="T20:AA20"/>
-    <mergeCell ref="T21:AA21"/>
-    <mergeCell ref="T12:AA12"/>
-    <mergeCell ref="T13:AA13"/>
-    <mergeCell ref="T14:AA14"/>
-    <mergeCell ref="T15:AA15"/>
-    <mergeCell ref="T16:AA16"/>
-    <mergeCell ref="T7:AA7"/>
-    <mergeCell ref="T8:AA8"/>
-    <mergeCell ref="T9:AA9"/>
-    <mergeCell ref="T10:AA10"/>
-    <mergeCell ref="T11:AA11"/>
-    <mergeCell ref="T26:AA26"/>
-    <mergeCell ref="Q33:AA33"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:J37"/>
+  <mergeCells count="46">
+    <mergeCell ref="A40:L41"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="N40:AA41"/>
+    <mergeCell ref="B28:V28"/>
+    <mergeCell ref="X28:Y28"/>
+    <mergeCell ref="B29:V29"/>
+    <mergeCell ref="F35:O35"/>
+    <mergeCell ref="F33:O33"/>
+    <mergeCell ref="F37:O37"/>
     <mergeCell ref="T5:AA6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:Y1"/>
@@ -3603,13 +3593,30 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="L3:Q3"/>
     <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="A40:L41"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="N40:AA41"/>
-    <mergeCell ref="B28:V28"/>
-    <mergeCell ref="X28:Y28"/>
-    <mergeCell ref="B29:V29"/>
-    <mergeCell ref="F35:O35"/>
+    <mergeCell ref="T26:AA26"/>
+    <mergeCell ref="Q33:AA33"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="T7:AA7"/>
+    <mergeCell ref="T8:AA8"/>
+    <mergeCell ref="T9:AA9"/>
+    <mergeCell ref="T10:AA10"/>
+    <mergeCell ref="T11:AA11"/>
+    <mergeCell ref="T12:AA12"/>
+    <mergeCell ref="T13:AA13"/>
+    <mergeCell ref="T14:AA14"/>
+    <mergeCell ref="T15:AA15"/>
+    <mergeCell ref="T16:AA16"/>
+    <mergeCell ref="T22:AA22"/>
+    <mergeCell ref="T23:AA23"/>
+    <mergeCell ref="T24:AA24"/>
+    <mergeCell ref="T25:AA25"/>
+    <mergeCell ref="T17:AA17"/>
+    <mergeCell ref="T18:AA18"/>
+    <mergeCell ref="T19:AA19"/>
+    <mergeCell ref="T20:AA20"/>
+    <mergeCell ref="T21:AA21"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="31" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
@@ -3619,6 +3626,33 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="8f42414a-44e9-4ab8-9d8c-13496e5456f0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5c5e1c5e-126c-46de-95d7-01837e6d0e6a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8f42414a-44e9-4ab8-9d8c-13496e5456f0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006FD7ECA55D469B4B85EC5E0598530405" ma:contentTypeVersion="19" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e424cba3a7cdf0ba8593dd1312d028ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8f42414a-44e9-4ab8-9d8c-13496e5456f0" xmlns:ns3="5c5e1c5e-126c-46de-95d7-01837e6d0e6a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b018def679fcf3d1e12496337ca2930" ns2:_="" ns3:_="">
     <xsd:import namespace="8f42414a-44e9-4ab8-9d8c-13496e5456f0"/>
@@ -3879,34 +3913,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="8f42414a-44e9-4ab8-9d8c-13496e5456f0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5c5e1c5e-126c-46de-95d7-01837e6d0e6a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8f42414a-44e9-4ab8-9d8c-13496e5456f0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBB2C939-EA99-47CE-A0FD-C18E0331C4D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D96C5256-C433-4124-8B9D-94EBEAE737AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8f42414a-44e9-4ab8-9d8c-13496e5456f0"/>
+    <ds:schemaRef ds:uri="5c5e1c5e-126c-46de-95d7-01837e6d0e6a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5550D66-634C-42C3-85ED-F122C19C87C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3923,23 +3949,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D96C5256-C433-4124-8B9D-94EBEAE737AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8f42414a-44e9-4ab8-9d8c-13496e5456f0"/>
-    <ds:schemaRef ds:uri="5c5e1c5e-126c-46de-95d7-01837e6d0e6a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBB2C939-EA99-47CE-A0FD-C18E0331C4D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>